<commit_message>
Update .DS_Store and AI_Risk_Assessment_Guide.xlsx
Minor updates to system files and Excel workbook after repository downloads

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/AI_Risk_Assessment_Guide.xlsx
+++ b/AI_Risk_Assessment_Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miachen/Desktop/Mia/DT Master/Tech/Hackthon/geminihackathon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135C3469-3049-A14F-A9DF-347F966F5165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008FE42F-02E9-F347-AD64-1DA2EB042C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8042,8 +8042,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8124,7 +8124,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="17" customFormat="1" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" s="17" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>289</v>
       </c>
@@ -8160,7 +8160,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>289</v>
       </c>
@@ -8199,7 +8199,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>289</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>289</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>289</v>
       </c>
@@ -8363,7 +8363,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>289</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -8446,7 +8446,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>154</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>154</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>154</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>154</v>
       </c>
@@ -8610,7 +8610,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>154</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>154</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>154</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>381</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>381</v>
       </c>
@@ -8862,7 +8862,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>381</v>
       </c>
@@ -8903,7 +8903,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>381</v>
       </c>
@@ -8985,7 +8985,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>381</v>
       </c>
@@ -9026,7 +9026,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>415</v>
       </c>
@@ -9067,7 +9067,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>415</v>
       </c>
@@ -9108,7 +9108,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>415</v>
       </c>
@@ -9149,7 +9149,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>415</v>
       </c>
@@ -9190,7 +9190,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>415</v>
       </c>
@@ -9231,7 +9231,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>415</v>
       </c>
@@ -9272,7 +9272,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>415</v>
       </c>
@@ -9313,7 +9313,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>415</v>
       </c>
@@ -9354,7 +9354,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>459</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>459</v>
       </c>
@@ -9436,7 +9436,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>459</v>
       </c>
@@ -9477,7 +9477,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>459</v>
       </c>
@@ -9518,7 +9518,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>459</v>
       </c>
@@ -9559,7 +9559,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>459</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>94</v>
       </c>
@@ -9682,7 +9682,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -9723,7 +9723,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>94</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -9852,7 +9852,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>528</v>
       </c>
@@ -9893,7 +9893,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>528</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>528</v>
       </c>
@@ -10016,7 +10016,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="48" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>528</v>
       </c>
@@ -10057,7 +10057,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>528</v>
       </c>
@@ -10098,7 +10098,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="50" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>528</v>
       </c>
@@ -10140,7 +10140,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="51" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>566</v>
       </c>
@@ -10181,7 +10181,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>566</v>
       </c>
@@ -10222,7 +10222,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>566</v>
       </c>
@@ -10263,7 +10263,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>566</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>566</v>
       </c>
@@ -10485,7 +10485,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>617</v>
       </c>
@@ -10527,7 +10527,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>617</v>
       </c>
@@ -10569,7 +10569,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>617</v>
       </c>
@@ -10608,7 +10608,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>617</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>617</v>
       </c>
@@ -10692,7 +10692,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>617</v>
       </c>
@@ -10784,7 +10784,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>661</v>
       </c>
@@ -10827,7 +10827,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>661</v>
       </c>
@@ -10923,7 +10923,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>661</v>
       </c>
@@ -10966,7 +10966,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>661</v>
       </c>
@@ -11005,7 +11005,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>691</v>
       </c>
@@ -11047,7 +11047,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>691</v>
       </c>
@@ -11089,7 +11089,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>691</v>
       </c>
@@ -11131,7 +11131,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>691</v>
       </c>
@@ -11372,7 +11372,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
         <v>739</v>
       </c>
@@ -11418,7 +11418,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
         <v>739</v>
       </c>
@@ -11516,7 +11516,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
         <v>739</v>
       </c>
@@ -11562,7 +11562,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
         <v>739</v>
       </c>
@@ -11608,7 +11608,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
         <v>739</v>
       </c>
@@ -11654,7 +11654,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
         <v>739</v>
       </c>
@@ -11752,7 +11752,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
         <v>739</v>
       </c>
@@ -11798,7 +11798,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
         <v>804</v>
       </c>
@@ -11842,7 +11842,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
         <v>804</v>
       </c>
@@ -11942,7 +11942,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
         <v>804</v>
       </c>
@@ -11988,7 +11988,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
         <v>804</v>
       </c>
@@ -12092,7 +12092,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
         <v>804</v>
       </c>
@@ -12300,7 +12300,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
         <v>804</v>
       </c>
@@ -12350,7 +12350,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
         <v>804</v>
       </c>
@@ -12452,7 +12452,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
         <v>804</v>
       </c>
@@ -12502,20 +12502,18 @@
         <v>893</v>
       </c>
     </row>
-    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F104" s="19"/>
       <c r="G104" s="19"/>
     </row>
-    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F105" s="19"/>
       <c r="G105" s="20"/>
       <c r="I105" s="19"/>
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
     </row>
-    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
       <c r="F106" s="19"/>
       <c r="G106" s="20"/>
       <c r="H106" s="48"/>
@@ -12523,7 +12521,7 @@
       <c r="J106" s="20"/>
       <c r="K106" s="19"/>
     </row>
-    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>894</v>
       </c>
@@ -12532,7 +12530,7 @@
       <c r="H107" s="48"/>
       <c r="I107" s="48"/>
     </row>
-    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>715</v>
       </c>
@@ -12545,7 +12543,7 @@
       <c r="I108" s="48"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>896</v>
       </c>
@@ -12559,7 +12557,7 @@
       <c r="J109" s="20"/>
       <c r="K109" s="19"/>
     </row>
-    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>898</v>
       </c>
@@ -12571,7 +12569,7 @@
       <c r="H110" s="48"/>
       <c r="I110" s="48"/>
     </row>
-    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>900</v>
       </c>
@@ -12584,7 +12582,7 @@
       <c r="I111" s="48"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>603</v>
       </c>
@@ -12598,7 +12596,7 @@
       <c r="J112" s="20"/>
       <c r="K112" s="19"/>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>594</v>
       </c>
@@ -12610,7 +12608,7 @@
       <c r="H113" s="48"/>
       <c r="I113" s="48"/>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>729</v>
       </c>
@@ -12621,7 +12619,7 @@
       <c r="I114" s="48"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>882</v>
       </c>
@@ -12633,96 +12631,175 @@
       <c r="J115" s="20"/>
       <c r="K115" s="19"/>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H116" s="48"/>
       <c r="I116" s="48"/>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H117" s="48"/>
       <c r="I117" s="48"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H118" s="48"/>
       <c r="I118" s="49"/>
       <c r="J118" s="20"/>
       <c r="K118" s="19"/>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H119" s="48"/>
       <c r="I119" s="48"/>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H120" s="48"/>
       <c r="I120" s="48"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H121" s="48"/>
       <c r="I121" s="49"/>
       <c r="J121" s="20"/>
       <c r="K121" s="19"/>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H122" s="48"/>
       <c r="I122" s="48"/>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H123" s="48"/>
       <c r="I123" s="48"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H124" s="48"/>
       <c r="I124" s="49"/>
       <c r="J124" s="20"/>
       <c r="K124" s="19"/>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H125" s="48"/>
       <c r="I125" s="48"/>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H126" s="48"/>
       <c r="I126" s="48"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H127" s="48"/>
       <c r="I127" s="49"/>
       <c r="J127" s="20"/>
       <c r="K127" s="19"/>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="H128" s="48"/>
       <c r="I128" s="48"/>
     </row>
-    <row r="129" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H129" s="48"/>
       <c r="I129" s="48"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H130" s="48"/>
       <c r="I130" s="49"/>
       <c r="J130" s="20"/>
       <c r="K130" s="19"/>
     </row>
-    <row r="131" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H131" s="48"/>
       <c r="I131" s="48"/>
     </row>
-    <row r="132" spans="8:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H132" s="48"/>
       <c r="I132" s="48"/>
       <c r="K132" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R132" xr:uid="{00000000-0001-0000-0300-000000000000}">
-    <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+    <filterColumn colId="11">
+      <filters blank="1">
+        <filter val="https://api.abuseipdb.com/api/v2/"/>
+        <filter val="https://api.electricitymap.org/"/>
+        <filter val="https://api.fda.gov/drug/event.json?limit=1"/>
+        <filter val="https://api.openai.com/v1/moderations"/>
+        <filter val="https://api.pwnedpasswords.com/"/>
+        <filter val="https://api.shodan.io/"/>
+        <filter val="https://api.ssllabs.com/api/v3/"/>
+        <filter val="https://api.thegreenwebfoundation.org/"/>
+        <filter val="https://api.websitecarbon.com/"/>
+        <filter val="https://ce-marking.help/"/>
+        <filter val="https://clinicaltables.nlm.nih.gov/api/"/>
+        <filter val="https://ec.europa.eu/"/>
+        <filter val="https://eur-lex.europa.eu/api"/>
+        <filter val="https://fhir.org/"/>
+        <filter val="https://flinkiso.com/"/>
+        <filter val="https://github.com/anchore/grype"/>
+        <filter val="https://github.com/anchore/syft"/>
+        <filter val="https://github.com/confident-ai/deepeval"/>
+        <filter val="https://github.com/dequelabs/axe-core"/>
+        <filter val="https://github.com/dssg/aequitas"/>
+        <filter val="https://github.com/evidentlyai/evidently"/>
+        <filter val="https://github.com/explodinggradients/ragas"/>
+        <filter val="https://github.com/explosion/spaCy"/>
+        <filter val="https://github.com/fairlearn/fairlearn"/>
+        <filter val="https://github.com/Hironsan/HateSonar"/>
+        <filter val="https://github.com/huggingface/evaluate"/>
+        <filter val="https://github.com/interpretml/interpret"/>
+        <filter val="https://github.com/joke2k/faker"/>
+        <filter val="https://github.com/marcotcr/lime"/>
+        <filter val="https://github.com/microsoft/presidio"/>
+        <filter val="https://github.com/mkdocs/mkdocs"/>
+        <filter val="https://github.com/mlco2/codecarbon"/>
+        <filter val="https://github.com/nexB/scancode-toolkit"/>
+        <filter val="https://github.com/opendp/opendp"/>
+        <filter val="https://github.com/ossf/scorecard"/>
+        <filter val="https://github.com/PAIR-code/what-if-tool"/>
+        <filter val="https://github.com/promptfoo/promptfoo"/>
+        <filter val="https://github.com/protectai/rebuff"/>
+        <filter val="https://github.com/pytorch/captum"/>
+        <filter val="https://github.com/pyupio/safety"/>
+        <filter val="https://github.com/SeldonIO/alibi-detect"/>
+        <filter val="https://github.com/sloria/TextBlob"/>
+        <filter val="https://github.com/slundberg/shap"/>
+        <filter val="https://github.com/TheHive-Project/TheHive"/>
+        <filter val="https://github.com/Trusted-AI/AIF360"/>
+        <filter val="https://github.com/uncertainty-toolbox/uncertainty-toolbox"/>
+        <filter val="https://github.com/unitaryai/detoxify"/>
+        <filter val="https://grafana.com/oss/grafana/"/>
+        <filter val="https://grafana.com/oss/loki/"/>
+        <filter val="https://huggingface.co/docs/hub/model-cards"/>
+        <filter val="https://hunter.io/"/>
+        <filter val="https://ico.org.uk/for-organisations/lawful-basis-interactive-guidance-tool/"/>
+        <filter val="https://ico.org.uk/for-organisations/uk-gdpr-guidance-and-resources/international-transfers/"/>
+        <filter val="https://idir.uta.edu/claimbuster/"/>
+        <filter val="https://idir.uta.edu/claimbuster/api/"/>
+        <filter val="https://kordon.app/gdpr-ropa-template/"/>
+        <filter val="https://mlco2.github.io/impact/"/>
+        <filter val="https://openethics.ai/label/"/>
+        <filter val="https://perspectiveapi.com/"/>
+        <filter val="https://services.nvd.nist.gov/rest/json/cves/2.0"/>
+        <filter val="https://smith.langchain.com/"/>
+        <filter val="https://snyk.io/"/>
+        <filter val="https://sourceforge.net/projects/opensourcepv/"/>
+        <filter val="https://spdx.org/licenses/"/>
+        <filter val="https://tineye.com/"/>
+        <filter val="https://transcend.io/"/>
+        <filter val="https://trustgdpa.com/free-tools/gdpr-fine-calculator/"/>
+        <filter val="https://urlhaus-api.abuse.ch/v1/"/>
+        <filter val="https://verifywise.ai/"/>
+        <filter val="https://wandb.ai/"/>
+        <filter val="https://www.cookiebot.com/"/>
+        <filter val="https://www.copyscape.com/"/>
+        <filter val="https://www.datagrail.io/"/>
+        <filter val="https://www.enforcementtracker.com/"/>
+        <filter val="https://www.hardenize.com/"/>
+        <filter val="https://www.humanrights.dk/tools/human-rights-impact-assessment-guidance-toolbox"/>
+        <filter val="https://www.onetrust.com/products/privacy-impact-assessment/"/>
+        <filter val="https://www.privacypolicies.com/"/>
+        <filter val="https://www.virustotal.com/api/v3/"/>
+        <filter val="N/A - Build Internally"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="18">

</xml_diff>